<commit_message>
first push of framework
</commit_message>
<xml_diff>
--- a/testdata/Odoodata.xlsx
+++ b/testdata/Odoodata.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="2472" windowWidth="18672" windowHeight="4104"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="124519"/>
+  <oleSize ref="A1:N26"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
   <si>
     <t>testcaseID</t>
   </si>
@@ -30,17 +31,74 @@
     <t>validLogin_ID</t>
   </si>
   <si>
-    <t>diganta.sdp@gmail.com</t>
-  </si>
-  <si>
-    <t>diganta27</t>
+    <t>Sector-14</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>Meera.Chopra@gamil.com</t>
+  </si>
+  <si>
+    <t>data4</t>
+  </si>
+  <si>
+    <t>data3</t>
+  </si>
+  <si>
+    <t>data5</t>
+  </si>
+  <si>
+    <t>data6</t>
+  </si>
+  <si>
+    <t>data7</t>
+  </si>
+  <si>
+    <t>data8</t>
+  </si>
+  <si>
+    <t>data9</t>
+  </si>
+  <si>
+    <t>data10</t>
+  </si>
+  <si>
+    <t>NehruPlace</t>
+  </si>
+  <si>
+    <t>Delhi</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>CustomersInfo</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>pratap.ganesh27@gmail.com</t>
+  </si>
+  <si>
+    <t>create_customer_ID</t>
+  </si>
+  <si>
+    <t>delete_customer_ID</t>
+  </si>
+  <si>
+    <t>Meera</t>
+  </si>
+  <si>
+    <t>Ganesh</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -103,8 +161,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -195,7 +255,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -230,7 +289,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -406,47 +464,67 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:11" s="3" customFormat="1">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>5</v>
+        <v>20</v>
+      </c>
+      <c r="C2" s="1">
+        <v>9755314363</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -457,24 +535,54 @@
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
+    <row r="3" spans="1:11">
+      <c r="A3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="1">
+        <v>9755314363</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3" s="1">
+        <v>201265</v>
+      </c>
+      <c r="J3" s="1">
+        <v>2415789944</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="1">
+        <v>9755314363</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
@@ -483,7 +591,7 @@
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -496,7 +604,7 @@
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -509,7 +617,7 @@
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -522,7 +630,7 @@
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -535,7 +643,7 @@
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -548,7 +656,7 @@
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -561,7 +669,7 @@
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -574,7 +682,7 @@
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -587,7 +695,7 @@
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -600,7 +708,7 @@
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -613,7 +721,7 @@
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -626,7 +734,7 @@
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -639,7 +747,7 @@
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -652,7 +760,7 @@
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -667,31 +775,69 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="K3" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId2"/>
+    <hyperlink ref="B3" r:id="rId3"/>
+    <hyperlink ref="B4" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
create and delete Customer
</commit_message>
<xml_diff>
--- a/testdata/Odoodata.xlsx
+++ b/testdata/Odoodata.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="14835" windowHeight="3465"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:K10"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
   <si>
     <t>testcaseID</t>
   </si>
@@ -30,16 +31,80 @@
     <t>validLogin_ID</t>
   </si>
   <si>
-    <t>diganta.sdp@gmail.com</t>
-  </si>
-  <si>
-    <t>diganta27</t>
+    <t>createCustomer_ID</t>
+  </si>
+  <si>
+    <t>data3</t>
+  </si>
+  <si>
+    <t>data4</t>
+  </si>
+  <si>
+    <t>data5</t>
+  </si>
+  <si>
+    <t>data6</t>
+  </si>
+  <si>
+    <t>data7</t>
+  </si>
+  <si>
+    <t>data8</t>
+  </si>
+  <si>
+    <t>street12</t>
+  </si>
+  <si>
+    <t>Noida</t>
+  </si>
+  <si>
+    <t>UttarPradesh</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>data9</t>
+  </si>
+  <si>
+    <t>data10</t>
+  </si>
+  <si>
+    <t>abc@gmail.com</t>
+  </si>
+  <si>
+    <t>pradeep7sah@gmail.com</t>
+  </si>
+  <si>
+    <t>sah5258u</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>prakash</t>
+  </si>
+  <si>
+    <t>Pradeep-11</t>
+  </si>
+  <si>
+    <t>Pradeep-575</t>
+  </si>
+  <si>
+    <t>deleteCustomer_ID</t>
+  </si>
+  <si>
+    <t>Pradeep-337</t>
+  </si>
+  <si>
+    <t>Pradeep-832</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -410,13 +475,17 @@
   <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="25.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -429,24 +498,40 @@
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
+      <c r="D1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -458,23 +543,53 @@
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="1">
+        <v>201301</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3" s="1">
+        <v>8956231478</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
+      <c r="A4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
@@ -485,7 +600,9 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
+      <c r="B5" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -667,7 +784,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="K3" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -675,12 +792,28 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Second push of FrameWork
</commit_message>
<xml_diff>
--- a/testdata/Odoodata.xlsx
+++ b/testdata/Odoodata.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t>testcaseID</t>
   </si>
@@ -58,13 +58,17 @@
     <t>sanu123456</t>
   </si>
   <si>
-    <t>deletecustomer_ID</t>
+    <t>Rock-26</t>
+  </si>
+  <si>
+    <t>Rock-26-820</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -130,13 +134,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -437,20 +442,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K18"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="24.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="22.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="21.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="4" customFormat="1">
@@ -491,7 +497,7 @@
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" customFormat="1">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -502,7 +508,7 @@
         <v>12</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>4</v>
@@ -526,13 +532,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
-      <c r="A4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>9</v>
-      </c>
+    <row r="4" spans="1:11" customFormat="1">
+      <c r="A4" s="1"/>
+      <c r="B4" s="6"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -541,11 +543,11 @@
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-    </row>
-    <row r="5" spans="1:11">
+      <c r="K4" s="2"/>
+    </row>
+    <row r="5" spans="1:11" customFormat="1">
       <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
+      <c r="B5" s="5"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -556,7 +558,7 @@
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" customFormat="1">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -569,7 +571,7 @@
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" customFormat="1">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -582,7 +584,7 @@
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" customFormat="1">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -595,7 +597,7 @@
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" customFormat="1">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -608,7 +610,7 @@
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" customFormat="1">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -621,7 +623,7 @@
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" customFormat="1">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -634,7 +636,7 @@
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" customFormat="1">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -647,7 +649,7 @@
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" customFormat="1">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -660,7 +662,7 @@
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" customFormat="1">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -673,7 +675,7 @@
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" customFormat="1">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -686,7 +688,7 @@
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" customFormat="1">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -699,7 +701,7 @@
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" customFormat="1">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -712,7 +714,7 @@
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" customFormat="1">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -724,6 +726,19 @@
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
+    </row>
+    <row r="19" spans="1:11" customFormat="1">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Third push of FrameWork
</commit_message>
<xml_diff>
--- a/testdata/Odoodata.xlsx
+++ b/testdata/Odoodata.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>testcaseID</t>
   </si>
@@ -58,10 +58,7 @@
     <t>sanu123456</t>
   </si>
   <si>
-    <t>Rock-26</t>
-  </si>
-  <si>
-    <t>Rock-26-820</t>
+    <t>Rock-539</t>
   </si>
 </sst>
 </file>
@@ -445,7 +442,7 @@
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -508,7 +505,7 @@
         <v>12</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
my day end puc
</commit_message>
<xml_diff>
--- a/testdata/Odoodata.xlsx
+++ b/testdata/Odoodata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16470" windowHeight="3060"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16335" windowHeight="3720"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="17">
   <si>
     <t>testcaseID</t>
   </si>
@@ -40,9 +40,6 @@
     <t>moejoe91</t>
   </si>
   <si>
-    <t>sharonH</t>
-  </si>
-  <si>
     <t>54 th ave.</t>
   </si>
   <si>
@@ -56,12 +53,28 @@
   </si>
   <si>
     <t>create customer_ID</t>
+  </si>
+  <si>
+    <t>sharonH-830-539-29</t>
+  </si>
+  <si>
+    <t>delete_customerID</t>
+  </si>
+  <si>
+    <t>sharonH-830-539-29-32</t>
+  </si>
+  <si>
+    <t>sharonH-830-539-29-32-859</t>
+  </si>
+  <si>
+    <t>sharonH-830-539-29-32-859-882</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -447,16 +460,16 @@
   <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="27.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="30.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -499,7 +512,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>5</v>
@@ -508,22 +521,22 @@
         <v>6</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="H3" s="1">
         <v>252881</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J3" s="1">
         <v>8987656766</v>
@@ -533,17 +546,39 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
+      <c r="A4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" s="1">
+        <v>252881</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J4" s="1">
+        <v>8987656766</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
@@ -732,6 +767,8 @@
     <hyperlink ref="K3" r:id="rId1"/>
     <hyperlink ref="B2" r:id="rId2"/>
     <hyperlink ref="B3" r:id="rId3"/>
+    <hyperlink ref="B4" r:id="rId4"/>
+    <hyperlink ref="K4" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
create salesteam and verified,delete salesteam and verified
</commit_message>
<xml_diff>
--- a/testdata/Odoodata.xlsx
+++ b/testdata/Odoodata.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
   <si>
     <t>testcaseID</t>
   </si>
@@ -46,28 +46,85 @@
     <t>ahtesham@gmail.com</t>
   </si>
   <si>
+    <t>createCustomer_ID</t>
+  </si>
+  <si>
+    <t>cool.sanu09@gmail.com</t>
+  </si>
+  <si>
+    <t>sanu123456</t>
+  </si>
+  <si>
+    <t>createSalesTeam_ID</t>
+  </si>
+  <si>
+    <t>Meeting</t>
+  </si>
+  <si>
+    <t>jason</t>
+  </si>
+  <si>
+    <t>jacson</t>
+  </si>
+  <si>
+    <t>jacson@gmail.com</t>
+  </si>
+  <si>
     <t>Rock</t>
   </si>
   <si>
-    <t>createCustomer_ID</t>
-  </si>
-  <si>
-    <t>cool.sanu09@gmail.com</t>
-  </si>
-  <si>
-    <t>sanu123456</t>
-  </si>
-  <si>
-    <t>Rock-539</t>
-  </si>
-  <si>
-    <t>Rock-539-345</t>
-  </si>
-  <si>
-    <t>Rock-539-345-161</t>
-  </si>
-  <si>
-    <t>Rock-539-345-161-19</t>
+    <t>Meeting-457</t>
+  </si>
+  <si>
+    <t>jacson-201</t>
+  </si>
+  <si>
+    <t>jacson@gmail.com-930</t>
+  </si>
+  <si>
+    <t>Meeting-457-544</t>
+  </si>
+  <si>
+    <t>jacson-201-605</t>
+  </si>
+  <si>
+    <t>jacson@gmail.com-930-27</t>
+  </si>
+  <si>
+    <t>Meeting-457-544-510</t>
+  </si>
+  <si>
+    <t>jacson-201-605-714</t>
+  </si>
+  <si>
+    <t>jacson@gmail.com-930-27-408</t>
+  </si>
+  <si>
+    <t>Meeting-457-544-510-346</t>
+  </si>
+  <si>
+    <t>jacson-201-605-714-949</t>
+  </si>
+  <si>
+    <t>jacson@gmail.com-930-27-408-594</t>
+  </si>
+  <si>
+    <t>Meeting-457-544-510-346-484</t>
+  </si>
+  <si>
+    <t>jacson-201-605-714-949-76</t>
+  </si>
+  <si>
+    <t>jacson@gmail.com-930-27-408-594-681</t>
+  </si>
+  <si>
+    <t>Meeting-457-544-510-346-484-30</t>
+  </si>
+  <si>
+    <t>jacson-201-605-714-949-76-152</t>
+  </si>
+  <si>
+    <t>jacson@gmail.com-930-27-408-594-681-945</t>
   </si>
 </sst>
 </file>
@@ -140,14 +197,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -451,7 +507,7 @@
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -461,6 +517,7 @@
     <col min="3" max="3" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
     <col min="5" max="5" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="16.42578125" collapsed="true"/>
     <col min="10" max="10" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
     <col min="11" max="11" bestFit="true" customWidth="true" width="21.0" collapsed="true"/>
   </cols>
@@ -489,10 +546,10 @@
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -505,16 +562,16 @@
     </row>
     <row r="3" spans="1:11" customFormat="1">
       <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="D3" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>4</v>
@@ -539,13 +596,27 @@
       </c>
     </row>
     <row r="4" spans="1:11" customFormat="1">
-      <c r="A4" s="1"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
+      <c r="A4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
@@ -749,9 +820,10 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="K3" r:id="rId1"/>
+    <hyperlink ref="F4" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Script:- salesteam create, delete and verified, opportunity create,verified and drag
</commit_message>
<xml_diff>
--- a/testdata/Odoodata.xlsx
+++ b/testdata/Odoodata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2472" windowWidth="18672" windowHeight="4356"/>
+    <workbookView xWindow="0" yWindow="2472" windowWidth="18456" windowHeight="8112"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
   <si>
     <t>testcaseID</t>
   </si>
@@ -67,34 +67,52 @@
     <t>pratap.ganesh27@gmail.com</t>
   </si>
   <si>
-    <t>delete_customer_ID</t>
+    <t>NehruPlace</t>
+  </si>
+  <si>
+    <t>Delhi</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>Meera.Chopra@gamil.com</t>
+  </si>
+  <si>
+    <t>create_customer_ID</t>
+  </si>
+  <si>
+    <t>create_salesTeam_ID</t>
+  </si>
+  <si>
+    <t>Meeting_Ganesh</t>
+  </si>
+  <si>
+    <t>Ganesh</t>
+  </si>
+  <si>
+    <t>Meeting</t>
+  </si>
+  <si>
+    <t>create_opportunity_ID</t>
+  </si>
+  <si>
+    <t>Ganesh@pratap.com</t>
+  </si>
+  <si>
+    <t>2200-MacBook</t>
   </si>
   <si>
     <t>Sector-14</t>
   </si>
   <si>
-    <t>NehruPlace</t>
-  </si>
-  <si>
-    <t>Delhi</t>
-  </si>
-  <si>
-    <t>India</t>
-  </si>
-  <si>
-    <t>Meera.Chopra@gamil.com</t>
-  </si>
-  <si>
-    <t>create_customer_ID</t>
-  </si>
-  <si>
-    <t>create_salesteam_ID</t>
-  </si>
-  <si>
-    <t>Meera</t>
-  </si>
-  <si>
-    <t>Meera-929</t>
+    <t>2200-MacBook-2</t>
+  </si>
+  <si>
+    <t>2200-MacBook-2-4</t>
+  </si>
+  <si>
+    <t>2200-MacBook-2-4-3</t>
   </si>
 </sst>
 </file>
@@ -469,21 +487,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K18"/>
+  <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="18.44140625" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="19.77734375" collapsed="true"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="25.109375" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="14.44140625" collapsed="true"/>
     <col min="5" max="5" customWidth="true" width="10.109375" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="11.109375" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="18.44140625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="14.77734375" collapsed="true"/>
     <col min="9" max="9" bestFit="true" customWidth="true" width="10.88671875" collapsed="true"/>
     <col min="10" max="10" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
     <col min="11" max="11" customWidth="true" width="24.33203125" collapsed="true"/>
@@ -545,7 +563,7 @@
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>15</v>
@@ -554,19 +572,19 @@
         <v>9755314363</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="I3" s="1">
         <v>201265</v>
@@ -575,12 +593,12 @@
         <v>2415789944</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="1" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>15</v>
@@ -591,9 +609,15 @@
       <c r="D4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
+      <c r="E4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
@@ -601,7 +625,7 @@
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>15</v>
@@ -609,8 +633,12 @@
       <c r="C5" s="1">
         <v>9755314363</v>
       </c>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
+      <c r="D5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" s="1">
+        <v>4500000</v>
+      </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
@@ -774,26 +802,14 @@
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
     </row>
-    <row r="18" spans="1:11">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
-      <c r="K18" s="1"/>
-    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="K3" r:id="rId1"/>
     <hyperlink ref="B2" r:id="rId2"/>
     <hyperlink ref="B3" r:id="rId3"/>
     <hyperlink ref="B4" r:id="rId4"/>
-    <hyperlink ref="B5" r:id="rId5"/>
+    <hyperlink ref="F4" r:id="rId5"/>
+    <hyperlink ref="B5" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
create salesteam, opportunity and activity
</commit_message>
<xml_diff>
--- a/testdata/Odoodata.xlsx
+++ b/testdata/Odoodata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="14835" windowHeight="3555"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="14835" windowHeight="6420"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
   <si>
     <t>testcaseID</t>
   </si>
@@ -28,9 +28,6 @@
     <t>CreateCustomer_ID</t>
   </si>
   <si>
-    <t>CreateOpportunityWithExitingCustomer_ID</t>
-  </si>
-  <si>
     <t>data1</t>
   </si>
   <si>
@@ -40,9 +37,6 @@
     <t>data2</t>
   </si>
   <si>
-    <t>Deep</t>
-  </si>
-  <si>
     <t>fashion Street</t>
   </si>
   <si>
@@ -61,7 +55,49 @@
     <t>deep@gmail.com</t>
   </si>
   <si>
-    <t>500 Keyboard</t>
+    <t>DeleteCustomer_ID</t>
+  </si>
+  <si>
+    <t>CreateOpportunity_ID</t>
+  </si>
+  <si>
+    <t>500 Keyboard and computer</t>
+  </si>
+  <si>
+    <t>CreatingSalesTeam_ID</t>
+  </si>
+  <si>
+    <t>pradeepsharma8850@gmail.com</t>
+  </si>
+  <si>
+    <t>SalesCall</t>
+  </si>
+  <si>
+    <t>SalesSMS</t>
+  </si>
+  <si>
+    <t>SalesMeeting</t>
+  </si>
+  <si>
+    <t>SalesTeam</t>
+  </si>
+  <si>
+    <t>Deep74</t>
+  </si>
+  <si>
+    <t>Sales965128</t>
+  </si>
+  <si>
+    <t>CreateActivity_ID</t>
+  </si>
+  <si>
+    <t>AutomationMeeting</t>
+  </si>
+  <si>
+    <t>Automation Meeting with Customer</t>
+  </si>
+  <si>
+    <t>Meeting</t>
   </si>
 </sst>
 </file>
@@ -114,11 +150,12 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -416,8 +453,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -425,9 +462,10 @@
     <col min="1" max="1" width="40.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="28.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="26.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="30.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="33.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="11" max="11" width="11" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="12" max="12" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
@@ -437,10 +475,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D1" s="3"/>
     </row>
@@ -449,7 +487,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2">
         <v>8527529100</v>
@@ -460,45 +498,45 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3">
         <v>8527529100</v>
       </c>
       <c r="D3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" t="s">
         <v>7</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G3" t="s">
         <v>8</v>
       </c>
-      <c r="F3" t="s">
+      <c r="H3" t="s">
         <v>9</v>
-      </c>
-      <c r="G3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H3" t="s">
-        <v>11</v>
       </c>
       <c r="I3">
         <v>110049</v>
       </c>
       <c r="J3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="K3">
         <v>7896541233</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:12">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C4">
         <v>8527529100</v>
@@ -506,8 +544,71 @@
       <c r="D4" t="s">
         <v>14</v>
       </c>
-      <c r="E4">
-        <v>10000</v>
+      <c r="E4" s="4">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>8527529100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>8527529100</v>
+      </c>
+      <c r="D6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" t="s">
+        <v>18</v>
+      </c>
+      <c r="I6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7">
+        <v>8527529100</v>
+      </c>
+      <c r="D7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G7" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="8:8">
@@ -519,8 +620,14 @@
     <hyperlink ref="B2" r:id="rId2"/>
     <hyperlink ref="B3" r:id="rId3"/>
     <hyperlink ref="L3" r:id="rId4"/>
+    <hyperlink ref="B5" r:id="rId5"/>
+    <hyperlink ref="B6" r:id="rId6"/>
+    <hyperlink ref="E6" r:id="rId7"/>
+    <hyperlink ref="B7" r:id="rId8"/>
+    <hyperlink ref="E7" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId10"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
importcustomer and salesteam and create opportuinity
</commit_message>
<xml_diff>
--- a/testdata/Odoodata.xlsx
+++ b/testdata/Odoodata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2472" windowWidth="11820" windowHeight="4188"/>
+    <workbookView xWindow="0" yWindow="2472" windowWidth="12120" windowHeight="3120"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="38">
   <si>
     <t>testcaseID</t>
   </si>
@@ -82,10 +82,55 @@
     <t>customersel_ID</t>
   </si>
   <si>
-    <t>harry-149</t>
-  </si>
-  <si>
-    <t>harry-126</t>
+    <t>pipeline_ID</t>
+  </si>
+  <si>
+    <t>100pendrive</t>
+  </si>
+  <si>
+    <t>shahzad</t>
+  </si>
+  <si>
+    <t>20000</t>
+  </si>
+  <si>
+    <t>salesteam_ID</t>
+  </si>
+  <si>
+    <t>achal</t>
+  </si>
+  <si>
+    <t>9211863489</t>
+  </si>
+  <si>
+    <t>sales:meeting</t>
+  </si>
+  <si>
+    <t>harry-120</t>
+  </si>
+  <si>
+    <t>abr16@gmail.com-2</t>
+  </si>
+  <si>
+    <t>nawazk-88</t>
+  </si>
+  <si>
+    <t>sadx182@gmai.com</t>
+  </si>
+  <si>
+    <t>ahetsamm-69</t>
+  </si>
+  <si>
+    <t>ahetsamm-31</t>
+  </si>
+  <si>
+    <t>abr16@gmail.com-20</t>
+  </si>
+  <si>
+    <t>nawazk-58</t>
+  </si>
+  <si>
+    <t>sadx182@gmai.com-10</t>
   </si>
 </sst>
 </file>
@@ -469,18 +514,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="22.6640625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="14.88671875" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="16.21875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="9.77734375" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="15.21875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="15.6640625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="20.33203125" collapsed="true"/>
+    <col min="8" max="9" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
     <col min="10" max="10" bestFit="true" customWidth="true" width="15.21875" collapsed="true"/>
   </cols>
   <sheetData>
@@ -574,7 +621,7 @@
         <v>20</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -587,10 +634,18 @@
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
+      <c r="A5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>24</v>
+      </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
@@ -600,14 +655,30 @@
       <c r="K5" s="1"/>
     </row>
     <row r="6" spans="1:11">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
+      <c r="A6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>27</v>
+      </c>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
@@ -774,9 +845,11 @@
     <hyperlink ref="D3" r:id="rId2" display="abc12@gmail.com"/>
     <hyperlink ref="B3" r:id="rId3"/>
     <hyperlink ref="J3" r:id="rId4"/>
+    <hyperlink ref="G6" r:id="rId5"/>
+    <hyperlink ref="D6" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
sales team created and deleted
</commit_message>
<xml_diff>
--- a/testdata/Odoodata.xlsx
+++ b/testdata/Odoodata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16335" windowHeight="3720"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15915" windowHeight="6060"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="33">
   <si>
     <t>testcaseID</t>
   </si>
@@ -55,19 +55,67 @@
     <t>create customer_ID</t>
   </si>
   <si>
-    <t>sharonH-830-539-29</t>
-  </si>
-  <si>
     <t>delete_customerID</t>
   </si>
   <si>
-    <t>sharonH-830-539-29-32</t>
-  </si>
-  <si>
-    <t>sharonH-830-539-29-32-859</t>
-  </si>
-  <si>
     <t>sharonH-830-539-29-32-859-882</t>
+  </si>
+  <si>
+    <t>createSalesTeam_ID</t>
+  </si>
+  <si>
+    <t>Email2</t>
+  </si>
+  <si>
+    <t>Kevin</t>
+  </si>
+  <si>
+    <t>sharonH-830-539-29-142</t>
+  </si>
+  <si>
+    <t>54 th ave.-930</t>
+  </si>
+  <si>
+    <t>Lakecity-795</t>
+  </si>
+  <si>
+    <t>100 macs</t>
+  </si>
+  <si>
+    <t>Kevin@gmail.com</t>
+  </si>
+  <si>
+    <t>clovis</t>
+  </si>
+  <si>
+    <t>createOpportunity_ID</t>
+  </si>
+  <si>
+    <t>Email2-778</t>
+  </si>
+  <si>
+    <t>Kevin-541</t>
+  </si>
+  <si>
+    <t>Kevin@gmail.com-516</t>
+  </si>
+  <si>
+    <t>Email2-778-764</t>
+  </si>
+  <si>
+    <t>Kevin-541-997</t>
+  </si>
+  <si>
+    <t>Kevin@gmail.com-516-662</t>
+  </si>
+  <si>
+    <t>Email2-778-764-955</t>
+  </si>
+  <si>
+    <t>Kevin-541-997-548</t>
+  </si>
+  <si>
+    <t>Kevin@gmail.com-516-662-668</t>
   </si>
 </sst>
 </file>
@@ -460,7 +508,7 @@
   <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -521,7 +569,7 @@
         <v>6</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>7</v>
@@ -547,7 +595,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>5</v>
@@ -556,13 +604,13 @@
         <v>6</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>9</v>
@@ -581,25 +629,51 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
+      <c r="A5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
+      <c r="I5" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
+      <c r="A6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="1">
+        <v>1000</v>
+      </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
@@ -769,6 +843,9 @@
     <hyperlink ref="B3" r:id="rId3"/>
     <hyperlink ref="B4" r:id="rId4"/>
     <hyperlink ref="K4" r:id="rId5"/>
+    <hyperlink ref="B5" r:id="rId6"/>
+    <hyperlink ref="B6" r:id="rId7"/>
+    <hyperlink ref="F5" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>